<commit_message>
Updating elnino-app blog contents
</commit_message>
<xml_diff>
--- a/blog/elnino-app/prob_vals.xlsx
+++ b/blog/elnino-app/prob_vals.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\llaumedr.IFR\Documents\LuisLauM.github.io\blog\elnino-app\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\InDemonic\Documents\LuisLauM.github.io\blog\elnino-app\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB40857A-CA45-41C5-B907-54AF511E8F6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE1CB5B6-3945-42EC-B575-B3FD27F88D04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-22212" yWindow="-108" windowWidth="22320" windowHeight="13176" xr2:uid="{E84E93AA-1F6F-422A-B619-73DFFD9A6158}"/>
+    <workbookView xWindow="38280" yWindow="-120" windowWidth="37710" windowHeight="21840" xr2:uid="{E84E93AA-1F6F-422A-B619-73DFFD9A6158}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -118,7 +118,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -128,6 +128,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -146,7 +147,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - Tema de 2022">
   <a:themeElements>
     <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
@@ -442,14 +443,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{645C29F5-28DB-4A95-A3F0-2FC922850167}">
-  <dimension ref="A1:S71"/>
+  <dimension ref="A1:S72"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A45" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A71" sqref="A71"/>
+      <selection pane="bottomLeft" activeCell="P72" sqref="P72"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.7109375" style="2" bestFit="1" customWidth="1"/>
   </cols>
@@ -2203,6 +2204,29 @@
         <v>2</v>
       </c>
     </row>
+    <row r="72" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A72" s="2">
+        <v>45702</v>
+      </c>
+      <c r="E72">
+        <v>49</v>
+      </c>
+      <c r="F72">
+        <v>51</v>
+      </c>
+      <c r="N72">
+        <v>7</v>
+      </c>
+      <c r="O72">
+        <v>53</v>
+      </c>
+      <c r="P72" s="5">
+        <v>35</v>
+      </c>
+      <c r="Q72">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="B1:J1"/>

</xml_diff>